<commit_message>
Added part to insert total and payable
</commit_message>
<xml_diff>
--- a/spreadsheet_parser/xlsx_files/copy/output_empty.xlsx
+++ b/spreadsheet_parser/xlsx_files/copy/output_empty.xlsx
@@ -363,131 +363,179 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 101</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>53.6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="D2" t="n">
-        <v>15.7</v>
+      <c r="B2" s="0" t="n">
+        <v>536</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>85.99999999999999</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="E2" t="n">
+        <v>778</v>
+      </c>
+      <c r="F2" t="n">
+        <v>389</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="2">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 118</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>120</v>
-      </c>
-      <c r="C3" t="n">
-        <v>55.6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>7.3</v>
+      <c r="B3" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>556</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>72.99999999999997</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1828</v>
+      </c>
+      <c r="F3" t="n">
+        <v>914</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="2">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 129</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>40.8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>24.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>11.8</v>
+      <c r="B4" s="0" t="n">
+        <v>408</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="E4" t="n">
+        <v>772</v>
+      </c>
+      <c r="F4" t="n">
+        <v>386</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="2">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 132</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>74.40000000000001</v>
-      </c>
-      <c r="C5" t="n">
-        <v>19.2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>35.2</v>
+      <c r="B5" s="0" t="n">
+        <v>743.9999999999999</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>352</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1287</v>
+      </c>
+      <c r="F5" t="n">
+        <v>643.5</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="2">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 156</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>9.6</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="B6" s="0" t="n">
+        <v>95.99999999999999</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>113</v>
+      </c>
+      <c r="F6" t="n">
+        <v>56.5</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="2">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 162</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>214.4</v>
-      </c>
-      <c r="C7" t="n">
-        <v>46.4</v>
-      </c>
-      <c r="D7" t="n">
-        <v>18.3</v>
+      <c r="B7" s="0" t="n">
+        <v>2144</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>464</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2791</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1395.5</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="2">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 165</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>98</v>
-      </c>
-      <c r="C8" t="n">
-        <v>30.6</v>
-      </c>
-      <c r="D8" t="n">
-        <v>54.5</v>
+      <c r="B8" s="0" t="n">
+        <v>980</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>306</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>545</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1831</v>
+      </c>
+      <c r="F8" t="n">
+        <v>915.5</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="2">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>Terrible's - 170</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>148.8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B9" s="0" t="n">
+        <v>1488</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1493</v>
+      </c>
+      <c r="F9" t="n">
+        <v>746.5</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="2"/>

</xml_diff>

<commit_message>
Refactored code to be modular and use callbacks to be able to publish lol
</commit_message>
<xml_diff>
--- a/spreadsheet_parser/xlsx_files/copy/output_empty.xlsx
+++ b/spreadsheet_parser/xlsx_files/copy/output_empty.xlsx
@@ -363,179 +363,179 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="2">
-      <c r="A2" s="0" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Terrible's - 101</t>
         </is>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>536</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>85.99999999999999</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>157</v>
+      <c r="B2" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15.7</v>
       </c>
       <c r="E2" t="n">
-        <v>778</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>389</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="2">
-      <c r="A3" s="0" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Terrible's - 118</t>
         </is>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>556</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>72.99999999999997</v>
+      <c r="B3" t="n">
+        <v>120</v>
+      </c>
+      <c r="C3" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7.3</v>
       </c>
       <c r="E3" t="n">
-        <v>1828</v>
+        <v>182.9</v>
       </c>
       <c r="F3" t="n">
-        <v>914</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="2">
-      <c r="A4" s="0" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Terrible's - 129</t>
         </is>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>408</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>246</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>118</v>
+      <c r="B4" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>11.8</v>
       </c>
       <c r="E4" t="n">
-        <v>772</v>
+        <v>77.2</v>
       </c>
       <c r="F4" t="n">
-        <v>386</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="2">
-      <c r="A5" s="0" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Terrible's - 132</t>
         </is>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>743.9999999999999</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>192</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>352</v>
+      <c r="B5" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>35.2</v>
       </c>
       <c r="E5" t="n">
-        <v>1287</v>
+        <v>128.8</v>
       </c>
       <c r="F5" t="n">
-        <v>643.5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="2">
-      <c r="A6" s="0" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Terrible's - 156</t>
         </is>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>95.99999999999999</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="B6" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>113</v>
+        <v>11.4</v>
       </c>
       <c r="F6" t="n">
-        <v>56.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="2">
-      <c r="A7" s="0" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Terrible's - 162</t>
         </is>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>2144</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>464</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>183</v>
+      <c r="B7" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>18.3</v>
       </c>
       <c r="E7" t="n">
-        <v>2791</v>
+        <v>279.1</v>
       </c>
       <c r="F7" t="n">
-        <v>1395.5</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="2">
-      <c r="A8" s="0" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Terrible's - 165</t>
         </is>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>980</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>306</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>545</v>
+      <c r="B8" t="n">
+        <v>98</v>
+      </c>
+      <c r="C8" t="n">
+        <v>30.6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>54.5</v>
       </c>
       <c r="E8" t="n">
-        <v>1831</v>
+        <v>183.1</v>
       </c>
       <c r="F8" t="n">
-        <v>915.5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="2">
-      <c r="A9" s="0" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Terrible's - 170</t>
         </is>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>1488</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D9" s="0" t="n">
+      <c r="B9" t="n">
+        <v>148.8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>1493</v>
+        <v>149.3</v>
       </c>
       <c r="F9" t="n">
-        <v>746.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="2"/>

</xml_diff>